<commit_message>
Mis à jour Corrélation
</commit_message>
<xml_diff>
--- a/scripts/Edouard/Correlation_matrix_ville.xlsx
+++ b/scripts/Edouard/Correlation_matrix_ville.xlsx
@@ -396,19 +396,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.401037379741703</v>
+        <v>0.493367024071237</v>
       </c>
       <c r="D2" t="n">
-        <v>0.669247944947023</v>
+        <v>0.659662165314355</v>
       </c>
       <c r="E2" t="n">
-        <v>0.757539923452363</v>
+        <v>0.770933069422289</v>
       </c>
       <c r="F2" t="n">
-        <v>0.684157008417548</v>
+        <v>0.549502247347733</v>
       </c>
       <c r="G2" t="n">
-        <v>0.341264876093749</v>
+        <v>0.217973605171083</v>
       </c>
     </row>
     <row r="3">
@@ -416,22 +416,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.401037379741703</v>
+        <v>0.493367024071237</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.641351182450788</v>
+        <v>0.551897196626651</v>
       </c>
       <c r="E3" t="n">
-        <v>0.328587475137172</v>
+        <v>0.447316253062892</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0104324534166673</v>
+        <v>-0.0655443226404276</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.219667613680824</v>
+        <v>-0.298608174491895</v>
       </c>
     </row>
     <row r="4">
@@ -439,22 +439,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.669247944947023</v>
+        <v>0.659662165314355</v>
       </c>
       <c r="C4" t="n">
-        <v>0.641351182450788</v>
+        <v>0.551897196626651</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.747630766075363</v>
+        <v>0.78361925100665</v>
       </c>
       <c r="F4" t="n">
-        <v>0.580352769542977</v>
+        <v>0.392488167211744</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0796205434817873</v>
+        <v>-0.12359513834032</v>
       </c>
     </row>
     <row r="5">
@@ -462,22 +462,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.757539923452363</v>
+        <v>0.770933069422289</v>
       </c>
       <c r="C5" t="n">
-        <v>0.328587475137172</v>
+        <v>0.447316253062892</v>
       </c>
       <c r="D5" t="n">
-        <v>0.747630766075363</v>
+        <v>0.78361925100665</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.651883755900176</v>
+        <v>0.55063452664881</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0741867862708555</v>
+        <v>-0.22625033920859</v>
       </c>
     </row>
     <row r="6">
@@ -485,22 +485,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.684157008417548</v>
+        <v>0.549502247347733</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0104324534166673</v>
+        <v>-0.0655443226404276</v>
       </c>
       <c r="D6" t="n">
-        <v>0.580352769542977</v>
+        <v>0.392488167211744</v>
       </c>
       <c r="E6" t="n">
-        <v>0.651883755900176</v>
+        <v>0.55063452664881</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.10127161935984</v>
+        <v>0.0668730984730335</v>
       </c>
     </row>
     <row r="7">
@@ -508,19 +508,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.341264876093749</v>
+        <v>0.217973605171083</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.219667613680824</v>
+        <v>-0.298608174491895</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0796205434817873</v>
+        <v>-0.12359513834032</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0741867862708555</v>
+        <v>-0.22625033920859</v>
       </c>
       <c r="F7" t="n">
-        <v>0.10127161935984</v>
+        <v>0.0668730984730335</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -571,19 +571,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.629906797741115</v>
+        <v>0.497973550996671</v>
       </c>
       <c r="D2" t="n">
-        <v>0.230305966374754</v>
+        <v>-0.0643901413606171</v>
       </c>
       <c r="E2" t="n">
-        <v>0.424446886131912</v>
+        <v>0.463761020727406</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.27904566152064</v>
+        <v>-0.331023633136514</v>
       </c>
       <c r="G2" t="n">
-        <v>0.551032284849136</v>
+        <v>0.542387538504438</v>
       </c>
     </row>
     <row r="3">
@@ -591,22 +591,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.629906797741115</v>
+        <v>0.497973550996671</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.591124837168934</v>
+        <v>0.190702768235947</v>
       </c>
       <c r="E3" t="n">
-        <v>0.373074435352605</v>
+        <v>0.508427566507527</v>
       </c>
       <c r="F3" t="n">
-        <v>0.301361729961415</v>
+        <v>0.505597673361365</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0349732365459067</v>
+        <v>0.0733371328413457</v>
       </c>
     </row>
     <row r="4">
@@ -614,22 +614,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.230305966374754</v>
+        <v>-0.0643901413606171</v>
       </c>
       <c r="C4" t="n">
-        <v>0.591124837168934</v>
+        <v>0.190702768235947</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.194076576508112</v>
+        <v>0.0458749036578238</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0761348154890387</v>
+        <v>0.0737230234435839</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.117990893270835</v>
+        <v>-0.0448196890732375</v>
       </c>
     </row>
     <row r="5">
@@ -637,22 +637,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.424446886131912</v>
+        <v>0.463761020727406</v>
       </c>
       <c r="C5" t="n">
-        <v>0.373074435352605</v>
+        <v>0.508427566507527</v>
       </c>
       <c r="D5" t="n">
-        <v>0.194076576508112</v>
+        <v>0.0458749036578238</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.171218274849337</v>
+        <v>0.262866408852198</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0100762008478625</v>
+        <v>0.0447915176767876</v>
       </c>
     </row>
     <row r="6">
@@ -660,22 +660,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.27904566152064</v>
+        <v>-0.331023633136514</v>
       </c>
       <c r="C6" t="n">
-        <v>0.301361729961415</v>
+        <v>0.505597673361365</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0761348154890387</v>
+        <v>0.0737230234435839</v>
       </c>
       <c r="E6" t="n">
-        <v>0.171218274849337</v>
+        <v>0.262866408852198</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.46239612027468</v>
+        <v>-0.434127752053819</v>
       </c>
     </row>
     <row r="7">
@@ -683,19 +683,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.551032284849136</v>
+        <v>0.542387538504438</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0349732365459067</v>
+        <v>0.0733371328413457</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.117990893270835</v>
+        <v>-0.0448196890732375</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0100762008478625</v>
+        <v>0.0447915176767876</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.46239612027468</v>
+        <v>-0.434127752053819</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>

</xml_diff>